<commit_message>
Practiced and used the Linux commands
</commit_message>
<xml_diff>
--- a/Linux 29-01-2026/Linux Commands.xlsx
+++ b/Linux 29-01-2026/Linux Commands.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gyana\Desktop\Linux-Lab\Linux 02-02-2026\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gyana\Desktop\Linux-Lab\Linux 29-01-2026\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D2891E2D-053D-4A91-9528-BBEBAC2857CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17FB1987-E8D2-4585-8E8E-8B8F02D0176D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A0B196E6-9042-42EA-A2B8-AE4936778805}"/>
   </bookViews>
@@ -40,7 +40,7 @@
   <metadataTypes count="1">
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
-  <futureMetadata name="XLRICHVALUE" count="28">
+  <futureMetadata name="XLRICHVALUE" count="33">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
@@ -237,8 +237,43 @@
         </ext>
       </extLst>
     </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="28"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="29"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="30"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="31"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="32"/>
+        </ext>
+      </extLst>
+    </bk>
   </futureMetadata>
-  <valueMetadata count="28">
+  <valueMetadata count="33">
     <bk>
       <rc t="1" v="0"/>
     </bk>
@@ -322,13 +357,28 @@
     </bk>
     <bk>
       <rc t="1" v="27"/>
+    </bk>
+    <bk>
+      <rc t="1" v="28"/>
+    </bk>
+    <bk>
+      <rc t="1" v="29"/>
+    </bk>
+    <bk>
+      <rc t="1" v="30"/>
+    </bk>
+    <bk>
+      <rc t="1" v="31"/>
+    </bk>
+    <bk>
+      <rc t="1" v="32"/>
     </bk>
   </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="73">
   <si>
     <t>Serial No.</t>
   </si>
@@ -517,6 +567,82 @@
   </si>
   <si>
     <t>cp olde_file_data new_file</t>
+  </si>
+  <si>
+    <t>To copy more than one file to another</t>
+  </si>
+  <si>
+    <t>cat file1 file2 &gt; new_file</t>
+  </si>
+  <si>
+    <t>To display the first 10lines of data from file</t>
+  </si>
+  <si>
+    <t>head file_name</t>
+  </si>
+  <si>
+    <t>To display the last 10lines of the data from file</t>
+  </si>
+  <si>
+    <t>tail file_name</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">To display the first </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>th line of the file</t>
+    </r>
+  </si>
+  <si>
+    <t>head -n 15 file_name</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">To display the last </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>th line of the file.</t>
+    </r>
+  </si>
+  <si>
+    <t>tail -n 12 file_name</t>
   </si>
 </sst>
 </file>
@@ -713,7 +839,7 @@
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="28">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="33">
   <rv s="0">
     <v>0</v>
     <v>5</v>
@@ -824,6 +950,26 @@
   </rv>
   <rv s="0">
     <v>27</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>28</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>29</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>30</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>31</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>32</v>
     <v>5</v>
   </rv>
 </rvData>
@@ -868,6 +1014,11 @@
   <rel r:id="rId26"/>
   <rel r:id="rId27"/>
   <rel r:id="rId28"/>
+  <rel r:id="rId29"/>
+  <rel r:id="rId30"/>
+  <rel r:id="rId31"/>
+  <rel r:id="rId32"/>
+  <rel r:id="rId33"/>
 </richValueRels>
 </file>
 
@@ -1188,10 +1339,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{334A7071-D5B3-4A1A-929F-744EAE906AE6}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.4" x14ac:dyDescent="0.3"/>
@@ -1633,6 +1784,76 @@
         <v>#VALUE!</v>
       </c>
     </row>
+    <row r="32" spans="1:4" ht="92.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
+        <v>31</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D32" s="2" t="e" vm="29">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="102.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
+        <v>32</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D33" s="2" t="e" vm="30">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="99" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
+        <v>33</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D34" s="2" t="e" vm="31">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="123.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <v>34</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D35" s="2" t="e" vm="32">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="102" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
+        <v>35</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D36" s="2" t="e" vm="33">
+        <v>#VALUE!</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>